<commit_message>
edit notification and reporting
</commit_message>
<xml_diff>
--- a/14010224-سرویس های موردنیاز شاپکس.xlsx
+++ b/14010224-سرویس های موردنیاز شاپکس.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tamrin\draw\postex diagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tamrin\draw\Documents\documents_diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3635C7A-6B1C-453A-841A-16B7EB17A5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E36459-D872-4A46-B922-04151B660672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2892" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="169">
   <si>
     <t>با توجه به بررسی های انجام شده، برای توسعه شاپکس، نیاز به تغییر جزئی در معماری است.
   - تغییر به .Net Core برای دستیابی به سرعت بیشتر در توسعه و اجرای کدها
@@ -423,9 +423,6 @@
     <t>routOPtimization</t>
   </si>
   <si>
-    <t>Reporting</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -433,12 +430,6 @@
   </si>
   <si>
     <t>Show Reports</t>
-  </si>
-  <si>
-    <t>این سرویس وظیفه، تهیه و نمایش گزارشات رو بر عهده خواهد داشت گزارشات هم در سمت مشتری و هم سمت بک آفیس خواهد بود، همچنین هرگونه امور مربوط به تسریع گزارشات و جلوگیری از مشکلات ناشی از گزارش گیری در این سیستم انجام خواهد شد</t>
-  </si>
-  <si>
-    <t>در سمت مشتری گزارش گیری تا حدی وجود دارد</t>
   </si>
   <si>
     <t>در حال حاضر سمت بک آفیس گزارشات مناسب موجود نیست</t>
@@ -462,23 +453,7 @@
     <t>Merg Reports</t>
   </si>
   <si>
-    <t>I/O</t>
-  </si>
-  <si>
-    <t>Per Need</t>
-  </si>
-  <si>
     <t>Bulk orders insert from Excel</t>
-  </si>
-  <si>
-    <t>در این سیستم انواع ورودی و خروجی های اکسل ، PDF، XML, JSON انجام خواهد شد تا در صورتی که تولید و انجام عملیات در این قسمت ها با ترافیک زیاد همراه بود مابقی سیستم ها دچار مشکل و ورود به صف و یا کندی شدید نشوند</t>
-  </si>
-  <si>
-    <t>کدهای مربوط به کار با IO موجود است 
-اما نیاز به Abstract کردن دارد</t>
-  </si>
-  <si>
-    <t>انتزاعی سازی</t>
   </si>
   <si>
     <t>Create Excel Outpot</t>
@@ -569,6 +544,16 @@
   </si>
   <si>
     <t>Create Invoice</t>
+  </si>
+  <si>
+    <t>این سرویس وظیفه، تهیه و نمایش گزارشات رو بر عهده خواهد داشت گزارشات هم در سمت مشتری و هم سمت بک آفیس خواهد بود، همچنین هرگونه امور مربوط به تسریع گزارشات و جلوگیری از مشکلات ناشی از گزارش گیری در این سیستم انجام خواهد شد. در این سیستم انواع ورودی و خروجی های اکسل ، PDF، XML, JSON انجام خواهد شد تا در صورتی که تولید و انجام عملیات در این قسمت ها با ترافیک زیاد همراه بود مابقی سیستم ها دچار مشکل و ورود به صف و یا کندی شدید نشوند</t>
+  </si>
+  <si>
+    <t>در سمت مشتری گزارش گیری تا حدی وجود دارد. کدهای مربوط به کار با IO موجود است 
+اما نیاز به Abstract کردن دارد</t>
+  </si>
+  <si>
+    <t>Reporting I/O</t>
   </si>
 </sst>
 </file>
@@ -967,23 +952,73 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -992,34 +1027,11 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1027,35 +1039,6 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1286,104 +1269,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="47"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1402,8 +1385,8 @@
   <dimension ref="A1:W1003"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1494,24 +1477,24 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="48" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="13"/>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
@@ -1529,16 +1512,16 @@
       <c r="W3" s="12"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="65"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
       <c r="D4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
@@ -1556,14 +1539,14 @@
       <c r="W4" s="12"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
       <c r="D5" s="13"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
       <c r="K5" s="11"/>
@@ -1581,14 +1564,14 @@
       <c r="W5" s="12"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="51"/>
       <c r="D6" s="13"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -1606,16 +1589,16 @@
       <c r="W6" s="12"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="65"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
       <c r="K7" s="11"/>
@@ -1633,14 +1616,14 @@
       <c r="W7" s="12"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
+      <c r="A8" s="77"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -1658,26 +1641,26 @@
       <c r="W8" s="12"/>
     </row>
     <row r="9" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
-        <v>172</v>
+      <c r="A9" s="59" t="s">
+        <v>164</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="58" t="s">
         <v>86</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="47" t="s">
+      <c r="E9" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
@@ -1695,16 +1678,16 @@
       <c r="W9" s="12"/>
     </row>
     <row r="10" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="69"/>
-      <c r="C10" s="69"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
       <c r="D10" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
@@ -1722,16 +1705,16 @@
       <c r="W10" s="12"/>
     </row>
     <row r="11" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
@@ -1749,14 +1732,14 @@
       <c r="W11" s="12"/>
     </row>
     <row r="12" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
       <c r="D12" s="13"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
@@ -1774,14 +1757,14 @@
       <c r="W12" s="12"/>
     </row>
     <row r="13" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
@@ -1799,14 +1782,14 @@
       <c r="W13" s="12"/>
     </row>
     <row r="14" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
       <c r="D14" s="13"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
@@ -1824,24 +1807,24 @@
       <c r="W14" s="12"/>
     </row>
     <row r="15" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="55" t="s">
+      <c r="A15" s="72"/>
+      <c r="B15" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="55" t="s">
+      <c r="C15" s="48" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49" t="s">
+      <c r="G15" s="61"/>
+      <c r="H15" s="61" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="11"/>
@@ -1861,16 +1844,16 @@
       <c r="W15" s="12"/>
     </row>
     <row r="16" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
       <c r="D16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="60"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="66"/>
       <c r="I16" s="11"/>
       <c r="J16" s="16"/>
       <c r="K16" s="11"/>
@@ -1888,16 +1871,16 @@
       <c r="W16" s="12"/>
     </row>
     <row r="17" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
       <c r="D17" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
       <c r="I17" s="11"/>
       <c r="J17" s="16"/>
       <c r="K17" s="11"/>
@@ -1915,16 +1898,16 @@
       <c r="W17" s="12"/>
     </row>
     <row r="18" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
+      <c r="A18" s="72"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="60"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="66"/>
       <c r="I18" s="11"/>
       <c r="J18" s="16"/>
       <c r="K18" s="11"/>
@@ -1942,16 +1925,16 @@
       <c r="W18" s="12"/>
     </row>
     <row r="19" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
+      <c r="A19" s="72"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
       <c r="D19" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="60"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="54"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
       <c r="I19" s="11"/>
       <c r="J19" s="16"/>
       <c r="K19" s="11"/>
@@ -1969,16 +1952,16 @@
       <c r="W19" s="12"/>
     </row>
     <row r="20" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
       <c r="D20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="60"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="54"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
       <c r="I20" s="11"/>
       <c r="J20" s="16"/>
       <c r="K20" s="11"/>
@@ -1996,16 +1979,16 @@
       <c r="W20" s="12"/>
     </row>
     <row r="21" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
+      <c r="A21" s="72"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
       <c r="I21" s="11"/>
       <c r="J21" s="16"/>
       <c r="K21" s="11"/>
@@ -2023,16 +2006,16 @@
       <c r="W21" s="12"/>
     </row>
     <row r="22" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
+      <c r="A22" s="72"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="60"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
       <c r="I22" s="11"/>
       <c r="J22" s="16"/>
       <c r="K22" s="11"/>
@@ -2050,16 +2033,16 @@
       <c r="W22" s="12"/>
     </row>
     <row r="23" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
+      <c r="A23" s="72"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
       <c r="D23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="60"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
       <c r="I23" s="11"/>
       <c r="J23" s="16"/>
       <c r="K23" s="11"/>
@@ -2077,16 +2060,16 @@
       <c r="W23" s="12"/>
     </row>
     <row r="24" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
       <c r="D24" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="60"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
       <c r="I24" s="11"/>
       <c r="J24" s="16"/>
       <c r="K24" s="11"/>
@@ -2104,16 +2087,16 @@
       <c r="W24" s="12"/>
     </row>
     <row r="25" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="60"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="66"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="66"/>
       <c r="I25" s="11"/>
       <c r="J25" s="16"/>
       <c r="K25" s="11"/>
@@ -2131,16 +2114,16 @@
       <c r="W25" s="12"/>
     </row>
     <row r="26" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
+      <c r="A26" s="72"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="60"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
       <c r="I26" s="11"/>
       <c r="J26" s="18"/>
       <c r="K26" s="11"/>
@@ -2158,16 +2141,16 @@
       <c r="W26" s="12"/>
     </row>
     <row r="27" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="60"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
       <c r="K27" s="11"/>
@@ -2185,16 +2168,16 @@
       <c r="W27" s="12"/>
     </row>
     <row r="28" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
       <c r="D28" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="60"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="66"/>
+      <c r="H28" s="66"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
       <c r="K28" s="11"/>
@@ -2212,16 +2195,16 @@
       <c r="W28" s="12"/>
     </row>
     <row r="29" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
+      <c r="A29" s="72"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="60"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="66"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
@@ -2239,16 +2222,16 @@
       <c r="W29" s="12"/>
     </row>
     <row r="30" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
+      <c r="A30" s="72"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
       <c r="K30" s="11"/>
@@ -2266,16 +2249,16 @@
       <c r="W30" s="12"/>
     </row>
     <row r="31" spans="1:23" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
       <c r="D31" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="60"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="66"/>
+      <c r="H31" s="66"/>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
@@ -2293,16 +2276,16 @@
       <c r="W31" s="12"/>
     </row>
     <row r="32" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
+      <c r="A32" s="72"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
       <c r="D32" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="61"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
@@ -2320,20 +2303,20 @@
       <c r="W32" s="12"/>
     </row>
     <row r="33" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
+      <c r="A33" s="72"/>
       <c r="B33" s="42"/>
       <c r="C33" s="43"/>
       <c r="D33" s="20" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F33" s="39" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G33" s="39" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H33" s="39"/>
       <c r="I33" s="11"/>
@@ -2353,20 +2336,20 @@
       <c r="W33" s="12"/>
     </row>
     <row r="34" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="75"/>
+      <c r="A34" s="72"/>
+      <c r="B34" s="55"/>
       <c r="C34" s="43"/>
       <c r="D34" s="6" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
-      <c r="E34" s="47" t="s">
-        <v>157</v>
+      <c r="E34" s="62" t="s">
+        <v>149</v>
       </c>
-      <c r="F34" s="49" t="s">
-        <v>158</v>
+      <c r="F34" s="61" t="s">
+        <v>150</v>
       </c>
-      <c r="G34" s="49"/>
-      <c r="H34" s="49"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
       <c r="K34" s="11"/>
@@ -2384,16 +2367,16 @@
       <c r="W34" s="12"/>
     </row>
     <row r="35" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="76"/>
+      <c r="A35" s="72"/>
+      <c r="B35" s="56"/>
       <c r="C35" s="43"/>
       <c r="D35" s="6" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
       <c r="I35" s="11"/>
       <c r="J35" s="18"/>
       <c r="K35" s="11"/>
@@ -2411,16 +2394,16 @@
       <c r="W35" s="12"/>
     </row>
     <row r="36" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
-      <c r="B36" s="76"/>
+      <c r="A36" s="72"/>
+      <c r="B36" s="56"/>
       <c r="C36" s="43"/>
       <c r="D36" s="6" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="62"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
       <c r="I36" s="11"/>
       <c r="J36" s="18"/>
       <c r="K36" s="11"/>
@@ -2438,16 +2421,16 @@
       <c r="W36" s="12"/>
     </row>
     <row r="37" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="B37" s="76"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="56"/>
       <c r="C37" s="43"/>
       <c r="D37" s="6" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
       <c r="I37" s="11"/>
       <c r="J37" s="11"/>
       <c r="K37" s="11"/>
@@ -2465,14 +2448,14 @@
       <c r="W37" s="12"/>
     </row>
     <row r="38" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
-      <c r="B38" s="76"/>
+      <c r="A38" s="72"/>
+      <c r="B38" s="56"/>
       <c r="C38" s="43"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="62"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
       <c r="I38" s="11"/>
       <c r="J38" s="11"/>
       <c r="K38" s="11"/>
@@ -2490,14 +2473,14 @@
       <c r="W38" s="12"/>
     </row>
     <row r="39" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="52"/>
-      <c r="B39" s="77"/>
+      <c r="A39" s="72"/>
+      <c r="B39" s="57"/>
       <c r="C39" s="43"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="63"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="50"/>
+      <c r="H39" s="50"/>
       <c r="I39" s="11"/>
       <c r="J39" s="18"/>
       <c r="K39" s="11"/>
@@ -2515,21 +2498,21 @@
       <c r="W39" s="12"/>
     </row>
     <row r="40" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="52"/>
+      <c r="A40" s="72"/>
       <c r="B40" s="41"/>
       <c r="C40" s="22"/>
       <c r="D40" s="13" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
-      <c r="E40" s="47" t="s">
-        <v>163</v>
+      <c r="E40" s="62" t="s">
+        <v>155</v>
       </c>
-      <c r="F40" s="49" t="s">
-        <v>164</v>
+      <c r="F40" s="61" t="s">
+        <v>156</v>
       </c>
       <c r="G40" s="39"/>
-      <c r="H40" s="49" t="s">
-        <v>165</v>
+      <c r="H40" s="61" t="s">
+        <v>157</v>
       </c>
       <c r="I40" s="11"/>
       <c r="J40" s="18"/>
@@ -2548,16 +2531,16 @@
       <c r="W40" s="12"/>
     </row>
     <row r="41" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="53"/>
+      <c r="A41" s="73"/>
       <c r="B41" s="40"/>
       <c r="C41" s="22"/>
       <c r="D41" s="13" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
-      <c r="E41" s="48"/>
-      <c r="F41" s="50"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="67"/>
       <c r="G41" s="40"/>
-      <c r="H41" s="50"/>
+      <c r="H41" s="67"/>
       <c r="I41" s="11"/>
       <c r="J41" s="18"/>
       <c r="K41" s="11"/>
@@ -2575,28 +2558,28 @@
       <c r="W41" s="12"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A42" s="64" t="s">
+      <c r="A42" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="55" t="s">
+      <c r="B42" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="55" t="s">
+      <c r="C42" s="48" t="s">
         <v>16</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="59" t="s">
+      <c r="E42" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="F42" s="49" t="s">
+      <c r="F42" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="G42" s="49" t="s">
+      <c r="G42" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="49"/>
+      <c r="H42" s="61"/>
       <c r="I42" s="11"/>
       <c r="J42" s="11"/>
       <c r="K42" s="11"/>
@@ -2614,16 +2597,16 @@
       <c r="W42" s="12"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A43" s="62"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="62"/>
+      <c r="A43" s="49"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E43" s="62"/>
-      <c r="F43" s="62"/>
-      <c r="G43" s="62"/>
-      <c r="H43" s="62"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="K43" s="11"/>
@@ -2641,16 +2624,16 @@
       <c r="W43" s="12"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A44" s="62"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="62"/>
+      <c r="A44" s="49"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
       <c r="D44" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E44" s="62"/>
-      <c r="F44" s="62"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="62"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
       <c r="I44" s="11"/>
       <c r="J44" s="11"/>
       <c r="K44" s="11"/>
@@ -2668,16 +2651,16 @@
       <c r="W44" s="12"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A45" s="62"/>
-      <c r="B45" s="62"/>
-      <c r="C45" s="62"/>
+      <c r="A45" s="49"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E45" s="62"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="62"/>
-      <c r="H45" s="62"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
       <c r="I45" s="11"/>
       <c r="J45" s="11"/>
       <c r="K45" s="11"/>
@@ -2695,16 +2678,16 @@
       <c r="W45" s="12"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A46" s="62"/>
-      <c r="B46" s="62"/>
-      <c r="C46" s="62"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
       <c r="D46" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="62"/>
-      <c r="F46" s="62"/>
-      <c r="G46" s="62"/>
-      <c r="H46" s="62"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
       <c r="I46" s="11"/>
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
@@ -2722,16 +2705,16 @@
       <c r="W46" s="12"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A47" s="62"/>
-      <c r="B47" s="62"/>
-      <c r="C47" s="62"/>
+      <c r="A47" s="49"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
       <c r="D47" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E47" s="62"/>
-      <c r="F47" s="62"/>
-      <c r="G47" s="62"/>
-      <c r="H47" s="62"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
       <c r="I47" s="11"/>
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
@@ -2749,16 +2732,16 @@
       <c r="W47" s="12"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A48" s="62"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="62"/>
+      <c r="A48" s="49"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
       <c r="D48" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E48" s="62"/>
-      <c r="F48" s="62"/>
-      <c r="G48" s="62"/>
-      <c r="H48" s="62"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
       <c r="I48" s="11"/>
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
@@ -2776,16 +2759,16 @@
       <c r="W48" s="12"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A49" s="63"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
+      <c r="A49" s="50"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
       <c r="D49" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="63"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
       <c r="I49" s="11"/>
       <c r="J49" s="11"/>
       <c r="K49" s="11"/>
@@ -2803,28 +2786,28 @@
       <c r="W49" s="12"/>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A50" s="64" t="s">
+      <c r="A50" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="55" t="s">
+      <c r="B50" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="55" t="s">
+      <c r="C50" s="48" t="s">
         <v>16</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="67" t="s">
+      <c r="E50" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="F50" s="49" t="s">
+      <c r="F50" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="G50" s="49" t="s">
+      <c r="G50" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="H50" s="49" t="s">
+      <c r="H50" s="61" t="s">
         <v>60</v>
       </c>
       <c r="I50" s="11"/>
@@ -2844,16 +2827,16 @@
       <c r="W50" s="12"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A51" s="62"/>
-      <c r="B51" s="62"/>
-      <c r="C51" s="62"/>
+      <c r="A51" s="49"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
       <c r="D51" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="62"/>
-      <c r="F51" s="62"/>
-      <c r="G51" s="62"/>
-      <c r="H51" s="62"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="49"/>
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
       <c r="K51" s="11"/>
@@ -2871,14 +2854,14 @@
       <c r="W51" s="12"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A52" s="62"/>
-      <c r="B52" s="62"/>
-      <c r="C52" s="62"/>
+      <c r="A52" s="49"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="62"/>
-      <c r="F52" s="62"/>
-      <c r="G52" s="62"/>
-      <c r="H52" s="62"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="49"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
@@ -2896,14 +2879,14 @@
       <c r="W52" s="12"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A53" s="62"/>
-      <c r="B53" s="62"/>
-      <c r="C53" s="62"/>
+      <c r="A53" s="49"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
       <c r="D53" s="6"/>
-      <c r="E53" s="62"/>
-      <c r="F53" s="62"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="62"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
       <c r="I53" s="11"/>
       <c r="J53" s="11"/>
       <c r="K53" s="11"/>
@@ -2921,16 +2904,16 @@
       <c r="W53" s="12"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A54" s="62"/>
-      <c r="B54" s="62"/>
-      <c r="C54" s="62"/>
+      <c r="A54" s="49"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
       <c r="D54" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E54" s="62"/>
-      <c r="F54" s="62"/>
-      <c r="G54" s="62"/>
-      <c r="H54" s="62"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
       <c r="I54" s="11"/>
       <c r="J54" s="11"/>
       <c r="K54" s="11"/>
@@ -2948,16 +2931,16 @@
       <c r="W54" s="12"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A55" s="62"/>
-      <c r="B55" s="62"/>
-      <c r="C55" s="62"/>
+      <c r="A55" s="49"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="49"/>
       <c r="D55" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E55" s="62"/>
-      <c r="F55" s="62"/>
-      <c r="G55" s="62"/>
-      <c r="H55" s="62"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
       <c r="I55" s="11"/>
       <c r="J55" s="11"/>
       <c r="K55" s="11"/>
@@ -2975,16 +2958,16 @@
       <c r="W55" s="12"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A56" s="63"/>
-      <c r="B56" s="63"/>
-      <c r="C56" s="63"/>
+      <c r="A56" s="50"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
       <c r="D56" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E56" s="63"/>
-      <c r="F56" s="63"/>
-      <c r="G56" s="63"/>
-      <c r="H56" s="63"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="50"/>
       <c r="I56" s="11"/>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
@@ -3002,28 +2985,28 @@
       <c r="W56" s="12"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A57" s="51" t="s">
+      <c r="A57" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="B57" s="55" t="s">
+      <c r="B57" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C57" s="55" t="s">
+      <c r="C57" s="48" t="s">
         <v>66</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E57" s="47" t="s">
+      <c r="E57" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="F57" s="49" t="s">
+      <c r="F57" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="G57" s="49" t="s">
+      <c r="G57" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="H57" s="49" t="s">
+      <c r="H57" s="61" t="s">
         <v>71</v>
       </c>
       <c r="I57" s="11"/>
@@ -3043,16 +3026,16 @@
       <c r="W57" s="12"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A58" s="62"/>
-      <c r="B58" s="62"/>
-      <c r="C58" s="62"/>
+      <c r="A58" s="49"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="49"/>
       <c r="D58" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E58" s="62"/>
-      <c r="F58" s="62"/>
-      <c r="G58" s="62"/>
-      <c r="H58" s="62"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
       <c r="I58" s="11"/>
       <c r="J58" s="11"/>
       <c r="K58" s="11"/>
@@ -3070,16 +3053,16 @@
       <c r="W58" s="12"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A59" s="62"/>
-      <c r="B59" s="62"/>
-      <c r="C59" s="62"/>
+      <c r="A59" s="49"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="49"/>
       <c r="D59" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E59" s="62"/>
-      <c r="F59" s="62"/>
-      <c r="G59" s="62"/>
-      <c r="H59" s="62"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="49"/>
       <c r="I59" s="11"/>
       <c r="J59" s="11"/>
       <c r="K59" s="11"/>
@@ -3097,14 +3080,14 @@
       <c r="W59" s="12"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A60" s="62"/>
-      <c r="B60" s="62"/>
-      <c r="C60" s="62"/>
+      <c r="A60" s="49"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="49"/>
       <c r="D60" s="20"/>
-      <c r="E60" s="62"/>
-      <c r="F60" s="62"/>
-      <c r="G60" s="62"/>
-      <c r="H60" s="62"/>
+      <c r="E60" s="49"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="49"/>
       <c r="I60" s="11"/>
       <c r="J60" s="11"/>
       <c r="K60" s="11"/>
@@ -3122,14 +3105,14 @@
       <c r="W60" s="12"/>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A61" s="62"/>
-      <c r="B61" s="62"/>
-      <c r="C61" s="62"/>
+      <c r="A61" s="49"/>
+      <c r="B61" s="49"/>
+      <c r="C61" s="49"/>
       <c r="D61" s="6"/>
-      <c r="E61" s="62"/>
-      <c r="F61" s="62"/>
-      <c r="G61" s="62"/>
-      <c r="H61" s="62"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
       <c r="I61" s="11"/>
       <c r="J61" s="11"/>
       <c r="K61" s="11"/>
@@ -3147,14 +3130,14 @@
       <c r="W61" s="12"/>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A62" s="63"/>
-      <c r="B62" s="63"/>
-      <c r="C62" s="63"/>
+      <c r="A62" s="50"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="50"/>
       <c r="D62" s="6"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="63"/>
-      <c r="H62" s="63"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="50"/>
+      <c r="G62" s="50"/>
+      <c r="H62" s="50"/>
       <c r="I62" s="11"/>
       <c r="J62" s="11"/>
       <c r="K62" s="11"/>
@@ -3172,28 +3155,28 @@
       <c r="W62" s="12"/>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A63" s="64" t="s">
+      <c r="A63" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="68" t="s">
+      <c r="B63" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C63" s="68" t="s">
+      <c r="C63" s="58" t="s">
         <v>76</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E63" s="67" t="s">
+      <c r="E63" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="F63" s="71" t="s">
+      <c r="F63" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="G63" s="49" t="s">
+      <c r="G63" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="H63" s="49" t="s">
+      <c r="H63" s="61" t="s">
         <v>81</v>
       </c>
       <c r="I63" s="11"/>
@@ -3213,16 +3196,16 @@
       <c r="W63" s="12"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A64" s="62"/>
-      <c r="B64" s="62"/>
-      <c r="C64" s="62"/>
+      <c r="A64" s="49"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="49"/>
       <c r="D64" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E64" s="62"/>
-      <c r="F64" s="62"/>
-      <c r="G64" s="62"/>
-      <c r="H64" s="62"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
       <c r="I64" s="11"/>
       <c r="J64" s="18"/>
       <c r="K64" s="11"/>
@@ -3240,16 +3223,16 @@
       <c r="W64" s="12"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A65" s="62"/>
-      <c r="B65" s="62"/>
-      <c r="C65" s="62"/>
+      <c r="A65" s="49"/>
+      <c r="B65" s="49"/>
+      <c r="C65" s="49"/>
       <c r="D65" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E65" s="62"/>
-      <c r="F65" s="62"/>
-      <c r="G65" s="62"/>
-      <c r="H65" s="62"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49"/>
       <c r="I65" s="11"/>
       <c r="J65" s="11"/>
       <c r="K65" s="11"/>
@@ -3267,16 +3250,16 @@
       <c r="W65" s="12"/>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A66" s="63"/>
-      <c r="B66" s="63"/>
-      <c r="C66" s="63"/>
+      <c r="A66" s="50"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="50"/>
       <c r="D66" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E66" s="63"/>
-      <c r="F66" s="63"/>
-      <c r="G66" s="63"/>
-      <c r="H66" s="63"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="50"/>
+      <c r="G66" s="50"/>
+      <c r="H66" s="50"/>
       <c r="I66" s="11"/>
       <c r="J66" s="11"/>
       <c r="K66" s="11"/>
@@ -3294,26 +3277,26 @@
       <c r="W66" s="12"/>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A67" s="51" t="s">
+      <c r="A67" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="B67" s="68" t="s">
+      <c r="B67" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="C67" s="68" t="s">
+      <c r="C67" s="58" t="s">
         <v>86</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="E67" s="47" t="s">
+      <c r="E67" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="F67" s="49" t="s">
+      <c r="F67" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="G67" s="49"/>
-      <c r="H67" s="49"/>
+      <c r="G67" s="61"/>
+      <c r="H67" s="61"/>
       <c r="I67" s="11"/>
       <c r="J67" s="11"/>
       <c r="K67" s="11"/>
@@ -3331,16 +3314,16 @@
       <c r="W67" s="12"/>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A68" s="62"/>
-      <c r="B68" s="62"/>
-      <c r="C68" s="62"/>
+      <c r="A68" s="49"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="49"/>
       <c r="D68" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
-      <c r="G68" s="62"/>
-      <c r="H68" s="62"/>
+      <c r="E68" s="49"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
       <c r="I68" s="11"/>
       <c r="J68" s="11"/>
       <c r="K68" s="11"/>
@@ -3358,16 +3341,16 @@
       <c r="W68" s="12"/>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A69" s="62"/>
-      <c r="B69" s="62"/>
-      <c r="C69" s="62"/>
+      <c r="A69" s="49"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="49"/>
       <c r="D69" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E69" s="62"/>
-      <c r="F69" s="62"/>
-      <c r="G69" s="62"/>
-      <c r="H69" s="62"/>
+      <c r="E69" s="49"/>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+      <c r="H69" s="49"/>
       <c r="I69" s="11"/>
       <c r="J69" s="11"/>
       <c r="K69" s="11"/>
@@ -3385,16 +3368,16 @@
       <c r="W69" s="12"/>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A70" s="62"/>
-      <c r="B70" s="62"/>
-      <c r="C70" s="62"/>
+      <c r="A70" s="49"/>
+      <c r="B70" s="49"/>
+      <c r="C70" s="49"/>
       <c r="D70" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E70" s="62"/>
-      <c r="F70" s="62"/>
-      <c r="G70" s="62"/>
-      <c r="H70" s="62"/>
+      <c r="E70" s="49"/>
+      <c r="F70" s="49"/>
+      <c r="G70" s="49"/>
+      <c r="H70" s="49"/>
       <c r="I70" s="11"/>
       <c r="J70" s="11"/>
       <c r="K70" s="11"/>
@@ -3412,16 +3395,16 @@
       <c r="W70" s="12"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A71" s="62"/>
-      <c r="B71" s="62"/>
-      <c r="C71" s="62"/>
+      <c r="A71" s="49"/>
+      <c r="B71" s="49"/>
+      <c r="C71" s="49"/>
       <c r="D71" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E71" s="62"/>
-      <c r="F71" s="62"/>
-      <c r="G71" s="62"/>
-      <c r="H71" s="62"/>
+      <c r="E71" s="49"/>
+      <c r="F71" s="49"/>
+      <c r="G71" s="49"/>
+      <c r="H71" s="49"/>
       <c r="I71" s="11"/>
       <c r="J71" s="11"/>
       <c r="K71" s="11"/>
@@ -3439,16 +3422,16 @@
       <c r="W71" s="12"/>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A72" s="63"/>
-      <c r="B72" s="63"/>
-      <c r="C72" s="63"/>
+      <c r="A72" s="50"/>
+      <c r="B72" s="50"/>
+      <c r="C72" s="50"/>
       <c r="D72" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E72" s="63"/>
-      <c r="F72" s="63"/>
-      <c r="G72" s="63"/>
-      <c r="H72" s="63"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="50"/>
+      <c r="G72" s="50"/>
+      <c r="H72" s="50"/>
       <c r="I72" s="11"/>
       <c r="J72" s="11"/>
       <c r="K72" s="11"/>
@@ -3466,28 +3449,28 @@
       <c r="W72" s="12"/>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A73" s="64" t="s">
+      <c r="A73" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="B73" s="68" t="s">
+      <c r="B73" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="58" t="s">
         <v>102</v>
       </c>
       <c r="D73" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="E73" s="59" t="s">
+      <c r="E73" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="F73" s="49" t="s">
+      <c r="F73" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="G73" s="49" t="s">
+      <c r="G73" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="H73" s="49" t="s">
+      <c r="H73" s="61" t="s">
         <v>105</v>
       </c>
       <c r="I73" s="11"/>
@@ -3507,16 +3490,16 @@
       <c r="W73" s="12"/>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A74" s="62"/>
-      <c r="B74" s="62"/>
-      <c r="C74" s="62"/>
+      <c r="A74" s="49"/>
+      <c r="B74" s="49"/>
+      <c r="C74" s="49"/>
       <c r="D74" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="E74" s="62"/>
-      <c r="F74" s="62"/>
-      <c r="G74" s="62"/>
-      <c r="H74" s="62"/>
+      <c r="E74" s="49"/>
+      <c r="F74" s="49"/>
+      <c r="G74" s="49"/>
+      <c r="H74" s="49"/>
       <c r="I74" s="11"/>
       <c r="J74" s="11"/>
       <c r="K74" s="11"/>
@@ -3534,16 +3517,16 @@
       <c r="W74" s="12"/>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A75" s="62"/>
-      <c r="B75" s="62"/>
-      <c r="C75" s="62"/>
+      <c r="A75" s="49"/>
+      <c r="B75" s="49"/>
+      <c r="C75" s="49"/>
       <c r="D75" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="E75" s="62"/>
-      <c r="F75" s="62"/>
-      <c r="G75" s="62"/>
-      <c r="H75" s="62"/>
+      <c r="E75" s="49"/>
+      <c r="F75" s="49"/>
+      <c r="G75" s="49"/>
+      <c r="H75" s="49"/>
       <c r="I75" s="11"/>
       <c r="J75" s="11"/>
       <c r="K75" s="11"/>
@@ -3561,14 +3544,14 @@
       <c r="W75" s="12"/>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A76" s="62"/>
-      <c r="B76" s="62"/>
-      <c r="C76" s="62"/>
+      <c r="A76" s="49"/>
+      <c r="B76" s="49"/>
+      <c r="C76" s="49"/>
       <c r="D76" s="19"/>
-      <c r="E76" s="62"/>
-      <c r="F76" s="62"/>
-      <c r="G76" s="62"/>
-      <c r="H76" s="62"/>
+      <c r="E76" s="49"/>
+      <c r="F76" s="49"/>
+      <c r="G76" s="49"/>
+      <c r="H76" s="49"/>
       <c r="I76" s="11"/>
       <c r="J76" s="11"/>
       <c r="K76" s="11"/>
@@ -3586,14 +3569,14 @@
       <c r="W76" s="12"/>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A77" s="62"/>
-      <c r="B77" s="62"/>
-      <c r="C77" s="62"/>
+      <c r="A77" s="49"/>
+      <c r="B77" s="49"/>
+      <c r="C77" s="49"/>
       <c r="D77" s="19"/>
-      <c r="E77" s="62"/>
-      <c r="F77" s="62"/>
-      <c r="G77" s="62"/>
-      <c r="H77" s="62"/>
+      <c r="E77" s="49"/>
+      <c r="F77" s="49"/>
+      <c r="G77" s="49"/>
+      <c r="H77" s="49"/>
       <c r="I77" s="11"/>
       <c r="J77" s="11"/>
       <c r="K77" s="11"/>
@@ -3611,14 +3594,14 @@
       <c r="W77" s="12"/>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A78" s="62"/>
-      <c r="B78" s="62"/>
-      <c r="C78" s="62"/>
+      <c r="A78" s="49"/>
+      <c r="B78" s="49"/>
+      <c r="C78" s="49"/>
       <c r="D78" s="19"/>
-      <c r="E78" s="62"/>
-      <c r="F78" s="62"/>
-      <c r="G78" s="62"/>
-      <c r="H78" s="62"/>
+      <c r="E78" s="49"/>
+      <c r="F78" s="49"/>
+      <c r="G78" s="49"/>
+      <c r="H78" s="49"/>
       <c r="I78" s="11"/>
       <c r="J78" s="11"/>
       <c r="K78" s="11"/>
@@ -3636,14 +3619,14 @@
       <c r="W78" s="12"/>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A79" s="63"/>
-      <c r="B79" s="63"/>
-      <c r="C79" s="63"/>
+      <c r="A79" s="50"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="50"/>
       <c r="D79" s="19"/>
-      <c r="E79" s="63"/>
-      <c r="F79" s="63"/>
-      <c r="G79" s="63"/>
-      <c r="H79" s="63"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="50"/>
+      <c r="G79" s="50"/>
+      <c r="H79" s="50"/>
       <c r="I79" s="11"/>
       <c r="J79" s="11"/>
       <c r="K79" s="11"/>
@@ -3661,26 +3644,26 @@
       <c r="W79" s="12"/>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A80" s="64" t="s">
+      <c r="A80" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="B80" s="72" t="s">
+      <c r="B80" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="C80" s="72" t="s">
+      <c r="C80" s="54" t="s">
         <v>110</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E80" s="67" t="s">
+      <c r="E80" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="F80" s="49" t="s">
+      <c r="F80" s="61" t="s">
         <v>113</v>
       </c>
-      <c r="G80" s="74"/>
-      <c r="H80" s="49" t="s">
+      <c r="G80" s="60"/>
+      <c r="H80" s="61" t="s">
         <v>114</v>
       </c>
       <c r="I80" s="11"/>
@@ -3700,16 +3683,16 @@
       <c r="W80" s="12"/>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A81" s="63"/>
-      <c r="B81" s="63"/>
-      <c r="C81" s="63"/>
+      <c r="A81" s="50"/>
+      <c r="B81" s="50"/>
+      <c r="C81" s="50"/>
       <c r="D81" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E81" s="63"/>
-      <c r="F81" s="63"/>
-      <c r="G81" s="63"/>
-      <c r="H81" s="63"/>
+      <c r="E81" s="50"/>
+      <c r="F81" s="50"/>
+      <c r="G81" s="50"/>
+      <c r="H81" s="50"/>
       <c r="I81" s="11"/>
       <c r="J81" s="11"/>
       <c r="K81" s="11"/>
@@ -3727,28 +3710,28 @@
       <c r="W81" s="12"/>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A82" s="64" t="s">
+      <c r="A82" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="B82" s="72" t="s">
+      <c r="B82" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="C82" s="72" t="s">
+      <c r="C82" s="54" t="s">
         <v>76</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="E82" s="47" t="s">
+      <c r="E82" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="F82" s="49" t="s">
+      <c r="F82" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="G82" s="49" t="s">
+      <c r="G82" s="61" t="s">
         <v>119</v>
       </c>
-      <c r="H82" s="49" t="s">
+      <c r="H82" s="61" t="s">
         <v>120</v>
       </c>
       <c r="I82" s="11"/>
@@ -3768,16 +3751,16 @@
       <c r="W82" s="12"/>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A83" s="62"/>
-      <c r="B83" s="62"/>
-      <c r="C83" s="62"/>
+      <c r="A83" s="49"/>
+      <c r="B83" s="49"/>
+      <c r="C83" s="49"/>
       <c r="D83" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E83" s="62"/>
-      <c r="F83" s="62"/>
-      <c r="G83" s="62"/>
-      <c r="H83" s="62"/>
+      <c r="E83" s="49"/>
+      <c r="F83" s="49"/>
+      <c r="G83" s="49"/>
+      <c r="H83" s="49"/>
       <c r="I83" s="11"/>
       <c r="J83" s="11"/>
       <c r="K83" s="11"/>
@@ -3795,16 +3778,16 @@
       <c r="W83" s="12"/>
     </row>
     <row r="84" spans="1:23" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A84" s="62"/>
-      <c r="B84" s="62"/>
-      <c r="C84" s="62"/>
+      <c r="A84" s="49"/>
+      <c r="B84" s="49"/>
+      <c r="C84" s="49"/>
       <c r="D84" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E84" s="62"/>
-      <c r="F84" s="62"/>
-      <c r="G84" s="62"/>
-      <c r="H84" s="62"/>
+      <c r="E84" s="49"/>
+      <c r="F84" s="49"/>
+      <c r="G84" s="49"/>
+      <c r="H84" s="49"/>
       <c r="I84" s="11"/>
       <c r="J84" s="11"/>
       <c r="K84" s="11"/>
@@ -3822,16 +3805,16 @@
       <c r="W84" s="12"/>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A85" s="62"/>
-      <c r="B85" s="62"/>
-      <c r="C85" s="62"/>
+      <c r="A85" s="49"/>
+      <c r="B85" s="49"/>
+      <c r="C85" s="49"/>
       <c r="D85" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E85" s="62"/>
-      <c r="F85" s="62"/>
-      <c r="G85" s="62"/>
-      <c r="H85" s="62"/>
+      <c r="E85" s="49"/>
+      <c r="F85" s="49"/>
+      <c r="G85" s="49"/>
+      <c r="H85" s="49"/>
       <c r="I85" s="11"/>
       <c r="J85" s="11"/>
       <c r="K85" s="11"/>
@@ -3849,16 +3832,16 @@
       <c r="W85" s="12"/>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A86" s="62"/>
-      <c r="B86" s="62"/>
-      <c r="C86" s="62"/>
+      <c r="A86" s="49"/>
+      <c r="B86" s="49"/>
+      <c r="C86" s="49"/>
       <c r="D86" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E86" s="62"/>
-      <c r="F86" s="62"/>
-      <c r="G86" s="62"/>
-      <c r="H86" s="62"/>
+      <c r="E86" s="49"/>
+      <c r="F86" s="49"/>
+      <c r="G86" s="49"/>
+      <c r="H86" s="49"/>
       <c r="I86" s="11"/>
       <c r="J86" s="11"/>
       <c r="K86" s="11"/>
@@ -3876,14 +3859,14 @@
       <c r="W86" s="12"/>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A87" s="63"/>
-      <c r="B87" s="63"/>
-      <c r="C87" s="63"/>
+      <c r="A87" s="50"/>
+      <c r="B87" s="50"/>
+      <c r="C87" s="50"/>
       <c r="D87" s="6"/>
-      <c r="E87" s="63"/>
-      <c r="F87" s="63"/>
-      <c r="G87" s="63"/>
-      <c r="H87" s="63"/>
+      <c r="E87" s="50"/>
+      <c r="F87" s="50"/>
+      <c r="G87" s="50"/>
+      <c r="H87" s="50"/>
       <c r="I87" s="11"/>
       <c r="J87" s="11"/>
       <c r="K87" s="11"/>
@@ -3901,29 +3884,29 @@
       <c r="W87" s="12"/>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A88" s="64" t="s">
+      <c r="A88" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="B88" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="B88" s="72" t="s">
+      <c r="C88" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="C88" s="72" t="s">
+      <c r="D88" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="D88" s="19" t="s">
+      <c r="E88" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="F88" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="G88" s="61" t="s">
         <v>128</v>
       </c>
-      <c r="E88" s="59" t="s">
+      <c r="H88" s="61" t="s">
         <v>129</v>
-      </c>
-      <c r="F88" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="G88" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="H88" s="49" t="s">
-        <v>132</v>
       </c>
       <c r="I88" s="11"/>
       <c r="J88" s="11"/>
@@ -3942,16 +3925,16 @@
       <c r="W88" s="12"/>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A89" s="62"/>
-      <c r="B89" s="62"/>
-      <c r="C89" s="62"/>
+      <c r="A89" s="49"/>
+      <c r="B89" s="49"/>
+      <c r="C89" s="49"/>
       <c r="D89" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
-      <c r="E89" s="62"/>
-      <c r="F89" s="62"/>
-      <c r="G89" s="62"/>
-      <c r="H89" s="62"/>
+      <c r="E89" s="49"/>
+      <c r="F89" s="49"/>
+      <c r="G89" s="49"/>
+      <c r="H89" s="49"/>
       <c r="I89" s="11"/>
       <c r="J89" s="11"/>
       <c r="K89" s="11"/>
@@ -3969,16 +3952,16 @@
       <c r="W89" s="12"/>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A90" s="62"/>
-      <c r="B90" s="62"/>
-      <c r="C90" s="62"/>
+      <c r="A90" s="49"/>
+      <c r="B90" s="49"/>
+      <c r="C90" s="49"/>
       <c r="D90" s="19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
-      <c r="E90" s="62"/>
-      <c r="F90" s="62"/>
-      <c r="G90" s="62"/>
-      <c r="H90" s="62"/>
+      <c r="E90" s="49"/>
+      <c r="F90" s="49"/>
+      <c r="G90" s="49"/>
+      <c r="H90" s="49"/>
       <c r="I90" s="11"/>
       <c r="J90" s="11"/>
       <c r="K90" s="11"/>
@@ -3996,16 +3979,16 @@
       <c r="W90" s="12"/>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A91" s="62"/>
-      <c r="B91" s="62"/>
-      <c r="C91" s="62"/>
+      <c r="A91" s="49"/>
+      <c r="B91" s="49"/>
+      <c r="C91" s="49"/>
       <c r="D91" s="19" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
-      <c r="E91" s="62"/>
-      <c r="F91" s="62"/>
-      <c r="G91" s="62"/>
-      <c r="H91" s="62"/>
+      <c r="E91" s="49"/>
+      <c r="F91" s="49"/>
+      <c r="G91" s="49"/>
+      <c r="H91" s="49"/>
       <c r="I91" s="11"/>
       <c r="J91" s="11"/>
       <c r="K91" s="11"/>
@@ -4023,16 +4006,16 @@
       <c r="W91" s="12"/>
     </row>
     <row r="92" spans="1:23" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="62"/>
-      <c r="B92" s="62"/>
-      <c r="C92" s="62"/>
+      <c r="A92" s="49"/>
+      <c r="B92" s="49"/>
+      <c r="C92" s="49"/>
       <c r="D92" s="19" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
-      <c r="E92" s="62"/>
-      <c r="F92" s="62"/>
-      <c r="G92" s="62"/>
-      <c r="H92" s="62"/>
+      <c r="E92" s="49"/>
+      <c r="F92" s="49"/>
+      <c r="G92" s="49"/>
+      <c r="H92" s="49"/>
       <c r="I92" s="27"/>
       <c r="J92" s="27"/>
       <c r="K92" s="27"/>
@@ -4050,16 +4033,16 @@
       <c r="W92" s="12"/>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A93" s="62"/>
-      <c r="B93" s="62"/>
-      <c r="C93" s="62"/>
+      <c r="A93" s="49"/>
+      <c r="B93" s="49"/>
+      <c r="C93" s="49"/>
       <c r="D93" s="19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
-      <c r="E93" s="62"/>
-      <c r="F93" s="62"/>
-      <c r="G93" s="62"/>
-      <c r="H93" s="62"/>
+      <c r="E93" s="49"/>
+      <c r="F93" s="49"/>
+      <c r="G93" s="49"/>
+      <c r="H93" s="49"/>
       <c r="I93" s="11"/>
       <c r="J93" s="11"/>
       <c r="K93" s="11"/>
@@ -4076,270 +4059,260 @@
       <c r="V93" s="12"/>
       <c r="W93" s="12"/>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A94" s="63"/>
-      <c r="B94" s="63"/>
-      <c r="C94" s="63"/>
+    <row r="94" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="49"/>
+      <c r="B94" s="49"/>
+      <c r="C94" s="49"/>
       <c r="D94" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E94" s="49"/>
+      <c r="F94" s="49"/>
+      <c r="G94" s="49"/>
+      <c r="H94" s="49"/>
+      <c r="I94" s="27"/>
+      <c r="J94" s="27"/>
+      <c r="K94" s="27"/>
+      <c r="L94" s="27"/>
+      <c r="M94" s="27"/>
+      <c r="N94" s="27"/>
+      <c r="O94" s="27"/>
+      <c r="P94" s="27"/>
+      <c r="Q94" s="27"/>
+      <c r="R94" s="27"/>
+      <c r="S94" s="27"/>
+      <c r="T94" s="27"/>
+      <c r="U94" s="27"/>
+      <c r="V94" s="12"/>
+      <c r="W94" s="12"/>
+    </row>
+    <row r="95" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="49"/>
+      <c r="B95" s="49"/>
+      <c r="C95" s="49"/>
+      <c r="D95" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E95" s="49"/>
+      <c r="F95" s="49"/>
+      <c r="G95" s="49"/>
+      <c r="H95" s="49"/>
+      <c r="I95" s="27"/>
+      <c r="J95" s="27"/>
+      <c r="K95" s="27"/>
+      <c r="L95" s="27"/>
+      <c r="M95" s="27"/>
+      <c r="N95" s="27"/>
+      <c r="O95" s="27"/>
+      <c r="P95" s="27"/>
+      <c r="Q95" s="27"/>
+      <c r="R95" s="27"/>
+      <c r="S95" s="27"/>
+      <c r="T95" s="27"/>
+      <c r="U95" s="27"/>
+      <c r="V95" s="12"/>
+      <c r="W95" s="12"/>
+    </row>
+    <row r="96" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="49"/>
+      <c r="B96" s="49"/>
+      <c r="C96" s="49"/>
+      <c r="D96" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E96" s="49"/>
+      <c r="F96" s="49"/>
+      <c r="G96" s="49"/>
+      <c r="H96" s="49"/>
+      <c r="I96" s="27"/>
+      <c r="J96" s="27"/>
+      <c r="K96" s="27"/>
+      <c r="L96" s="27"/>
+      <c r="M96" s="27"/>
+      <c r="N96" s="27"/>
+      <c r="O96" s="27"/>
+      <c r="P96" s="27"/>
+      <c r="Q96" s="27"/>
+      <c r="R96" s="27"/>
+      <c r="S96" s="27"/>
+      <c r="T96" s="27"/>
+      <c r="U96" s="27"/>
+      <c r="V96" s="12"/>
+      <c r="W96" s="12"/>
+    </row>
+    <row r="97" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="49"/>
+      <c r="B97" s="49"/>
+      <c r="C97" s="49"/>
+      <c r="D97" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E94" s="63"/>
-      <c r="F94" s="63"/>
-      <c r="G94" s="63"/>
-      <c r="H94" s="63"/>
-      <c r="I94" s="11"/>
-      <c r="J94" s="11"/>
-      <c r="K94" s="11"/>
-      <c r="L94" s="11"/>
-      <c r="M94" s="11"/>
-      <c r="N94" s="11"/>
-      <c r="O94" s="11"/>
-      <c r="P94" s="11"/>
-      <c r="Q94" s="11"/>
-      <c r="R94" s="11"/>
-      <c r="S94" s="11"/>
-      <c r="T94" s="11"/>
-      <c r="U94" s="11"/>
-      <c r="V94" s="12"/>
-      <c r="W94" s="12"/>
-    </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A95" s="64" t="s">
+      <c r="E97" s="49"/>
+      <c r="F97" s="49"/>
+      <c r="G97" s="49"/>
+      <c r="H97" s="49"/>
+      <c r="I97" s="27"/>
+      <c r="J97" s="27"/>
+      <c r="K97" s="27"/>
+      <c r="L97" s="27"/>
+      <c r="M97" s="27"/>
+      <c r="N97" s="27"/>
+      <c r="O97" s="27"/>
+      <c r="P97" s="27"/>
+      <c r="Q97" s="27"/>
+      <c r="R97" s="27"/>
+      <c r="S97" s="27"/>
+      <c r="T97" s="27"/>
+      <c r="U97" s="27"/>
+      <c r="V97" s="12"/>
+      <c r="W97" s="12"/>
+    </row>
+    <row r="98" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="49"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="49"/>
+      <c r="D98" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="B95" s="73" t="s">
+      <c r="E98" s="49"/>
+      <c r="F98" s="49"/>
+      <c r="G98" s="49"/>
+      <c r="H98" s="49"/>
+      <c r="I98" s="27"/>
+      <c r="J98" s="27"/>
+      <c r="K98" s="27"/>
+      <c r="L98" s="27"/>
+      <c r="M98" s="27"/>
+      <c r="N98" s="27"/>
+      <c r="O98" s="27"/>
+      <c r="P98" s="27"/>
+      <c r="Q98" s="27"/>
+      <c r="R98" s="27"/>
+      <c r="S98" s="27"/>
+      <c r="T98" s="27"/>
+      <c r="U98" s="27"/>
+      <c r="V98" s="12"/>
+      <c r="W98" s="12"/>
+    </row>
+    <row r="99" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="49"/>
+      <c r="B99" s="49"/>
+      <c r="C99" s="49"/>
+      <c r="D99" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C95" s="73"/>
-      <c r="D95" s="6" t="s">
+      <c r="E99" s="49"/>
+      <c r="F99" s="49"/>
+      <c r="G99" s="49"/>
+      <c r="H99" s="49"/>
+      <c r="I99" s="27"/>
+      <c r="J99" s="27"/>
+      <c r="K99" s="27"/>
+      <c r="L99" s="27"/>
+      <c r="M99" s="27"/>
+      <c r="N99" s="27"/>
+      <c r="O99" s="27"/>
+      <c r="P99" s="27"/>
+      <c r="Q99" s="27"/>
+      <c r="R99" s="27"/>
+      <c r="S99" s="27"/>
+      <c r="T99" s="27"/>
+      <c r="U99" s="27"/>
+      <c r="V99" s="12"/>
+      <c r="W99" s="12"/>
+    </row>
+    <row r="100" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="49"/>
+      <c r="B100" s="49"/>
+      <c r="C100" s="49"/>
+      <c r="D100" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="E95" s="67" t="s">
+      <c r="E100" s="49"/>
+      <c r="F100" s="49"/>
+      <c r="G100" s="49"/>
+      <c r="H100" s="49"/>
+      <c r="I100" s="27"/>
+      <c r="J100" s="27"/>
+      <c r="K100" s="27"/>
+      <c r="L100" s="27"/>
+      <c r="M100" s="27"/>
+      <c r="N100" s="27"/>
+      <c r="O100" s="27"/>
+      <c r="P100" s="27"/>
+      <c r="Q100" s="27"/>
+      <c r="R100" s="27"/>
+      <c r="S100" s="27"/>
+      <c r="T100" s="27"/>
+      <c r="U100" s="27"/>
+      <c r="V100" s="12"/>
+      <c r="W100" s="12"/>
+    </row>
+    <row r="101" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="49"/>
+      <c r="B101" s="49"/>
+      <c r="C101" s="49"/>
+      <c r="D101" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="F95" s="49" t="s">
+      <c r="E101" s="49"/>
+      <c r="F101" s="49"/>
+      <c r="G101" s="49"/>
+      <c r="H101" s="49"/>
+      <c r="I101" s="27"/>
+      <c r="J101" s="27"/>
+      <c r="K101" s="27"/>
+      <c r="L101" s="27"/>
+      <c r="M101" s="27"/>
+      <c r="N101" s="27"/>
+      <c r="O101" s="27"/>
+      <c r="P101" s="27"/>
+      <c r="Q101" s="27"/>
+      <c r="R101" s="27"/>
+      <c r="S101" s="27"/>
+      <c r="T101" s="27"/>
+      <c r="U101" s="27"/>
+      <c r="V101" s="12"/>
+      <c r="W101" s="12"/>
+    </row>
+    <row r="102" spans="1:23" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="49"/>
+      <c r="B102" s="49"/>
+      <c r="C102" s="49"/>
+      <c r="D102" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="G95" s="49"/>
-      <c r="H95" s="49" t="s">
+      <c r="E102" s="49"/>
+      <c r="F102" s="49"/>
+      <c r="G102" s="49"/>
+      <c r="H102" s="49"/>
+      <c r="I102" s="27"/>
+      <c r="J102" s="27"/>
+      <c r="K102" s="27"/>
+      <c r="L102" s="27"/>
+      <c r="M102" s="27"/>
+      <c r="N102" s="27"/>
+      <c r="O102" s="27"/>
+      <c r="P102" s="27"/>
+      <c r="Q102" s="27"/>
+      <c r="R102" s="27"/>
+      <c r="S102" s="27"/>
+      <c r="T102" s="27"/>
+      <c r="U102" s="27"/>
+      <c r="V102" s="12"/>
+      <c r="W102" s="12"/>
+    </row>
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A103" s="50"/>
+      <c r="B103" s="50"/>
+      <c r="C103" s="50"/>
+      <c r="D103" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="I95" s="11"/>
-      <c r="J95" s="11"/>
-      <c r="K95" s="11"/>
-      <c r="L95" s="11"/>
-      <c r="M95" s="11"/>
-      <c r="N95" s="11"/>
-      <c r="O95" s="11"/>
-      <c r="P95" s="11"/>
-      <c r="Q95" s="11"/>
-      <c r="R95" s="11"/>
-      <c r="S95" s="11"/>
-      <c r="T95" s="11"/>
-      <c r="U95" s="11"/>
-      <c r="V95" s="12"/>
-      <c r="W95" s="12"/>
-    </row>
-    <row r="96" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="62"/>
-      <c r="B96" s="62"/>
-      <c r="C96" s="62"/>
-      <c r="D96" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="E96" s="62"/>
-      <c r="F96" s="62"/>
-      <c r="G96" s="62"/>
-      <c r="H96" s="62"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="11"/>
-      <c r="K96" s="11"/>
-      <c r="L96" s="11"/>
-      <c r="M96" s="11"/>
-      <c r="N96" s="11"/>
-      <c r="O96" s="11"/>
-      <c r="P96" s="11"/>
-      <c r="Q96" s="11"/>
-      <c r="R96" s="11"/>
-      <c r="S96" s="11"/>
-      <c r="T96" s="11"/>
-      <c r="U96" s="11"/>
-      <c r="V96" s="12"/>
-      <c r="W96" s="12"/>
-    </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A97" s="62"/>
-      <c r="B97" s="62"/>
-      <c r="C97" s="62"/>
-      <c r="D97" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E97" s="62"/>
-      <c r="F97" s="62"/>
-      <c r="G97" s="62"/>
-      <c r="H97" s="62"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="11"/>
-      <c r="K97" s="11"/>
-      <c r="L97" s="11"/>
-      <c r="M97" s="11"/>
-      <c r="N97" s="11"/>
-      <c r="O97" s="11"/>
-      <c r="P97" s="11"/>
-      <c r="Q97" s="11"/>
-      <c r="R97" s="11"/>
-      <c r="S97" s="11"/>
-      <c r="T97" s="11"/>
-      <c r="U97" s="11"/>
-      <c r="V97" s="12"/>
-      <c r="W97" s="12"/>
-    </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A98" s="62"/>
-      <c r="B98" s="62"/>
-      <c r="C98" s="62"/>
-      <c r="D98" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E98" s="62"/>
-      <c r="F98" s="62"/>
-      <c r="G98" s="62"/>
-      <c r="H98" s="62"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
-      <c r="K98" s="11"/>
-      <c r="L98" s="11"/>
-      <c r="M98" s="11"/>
-      <c r="N98" s="11"/>
-      <c r="O98" s="11"/>
-      <c r="P98" s="11"/>
-      <c r="Q98" s="11"/>
-      <c r="R98" s="11"/>
-      <c r="S98" s="11"/>
-      <c r="T98" s="11"/>
-      <c r="U98" s="11"/>
-      <c r="V98" s="12"/>
-      <c r="W98" s="12"/>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A99" s="62"/>
-      <c r="B99" s="62"/>
-      <c r="C99" s="62"/>
-      <c r="D99" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E99" s="62"/>
-      <c r="F99" s="62"/>
-      <c r="G99" s="62"/>
-      <c r="H99" s="62"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="11"/>
-      <c r="K99" s="11"/>
-      <c r="L99" s="11"/>
-      <c r="M99" s="11"/>
-      <c r="N99" s="11"/>
-      <c r="O99" s="11"/>
-      <c r="P99" s="11"/>
-      <c r="Q99" s="11"/>
-      <c r="R99" s="11"/>
-      <c r="S99" s="11"/>
-      <c r="T99" s="11"/>
-      <c r="U99" s="11"/>
-      <c r="V99" s="12"/>
-      <c r="W99" s="12"/>
-    </row>
-    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A100" s="62"/>
-      <c r="B100" s="62"/>
-      <c r="C100" s="62"/>
-      <c r="D100" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E100" s="62"/>
-      <c r="F100" s="62"/>
-      <c r="G100" s="62"/>
-      <c r="H100" s="62"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="11"/>
-      <c r="K100" s="11"/>
-      <c r="L100" s="11"/>
-      <c r="M100" s="11"/>
-      <c r="N100" s="11"/>
-      <c r="O100" s="11"/>
-      <c r="P100" s="11"/>
-      <c r="Q100" s="11"/>
-      <c r="R100" s="11"/>
-      <c r="S100" s="11"/>
-      <c r="T100" s="11"/>
-      <c r="U100" s="11"/>
-      <c r="V100" s="12"/>
-      <c r="W100" s="12"/>
-    </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A101" s="62"/>
-      <c r="B101" s="62"/>
-      <c r="C101" s="62"/>
-      <c r="D101" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E101" s="62"/>
-      <c r="F101" s="62"/>
-      <c r="G101" s="62"/>
-      <c r="H101" s="62"/>
-      <c r="I101" s="11"/>
-      <c r="J101" s="11"/>
-      <c r="K101" s="11"/>
-      <c r="L101" s="11"/>
-      <c r="M101" s="11"/>
-      <c r="N101" s="11"/>
-      <c r="O101" s="11"/>
-      <c r="P101" s="11"/>
-      <c r="Q101" s="11"/>
-      <c r="R101" s="11"/>
-      <c r="S101" s="11"/>
-      <c r="T101" s="11"/>
-      <c r="U101" s="11"/>
-      <c r="V101" s="12"/>
-      <c r="W101" s="12"/>
-    </row>
-    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A102" s="62"/>
-      <c r="B102" s="62"/>
-      <c r="C102" s="62"/>
-      <c r="D102" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E102" s="62"/>
-      <c r="F102" s="62"/>
-      <c r="G102" s="62"/>
-      <c r="H102" s="62"/>
-      <c r="I102" s="11"/>
-      <c r="J102" s="11"/>
-      <c r="K102" s="11"/>
-      <c r="L102" s="11"/>
-      <c r="M102" s="11"/>
-      <c r="N102" s="11"/>
-      <c r="O102" s="11"/>
-      <c r="P102" s="11"/>
-      <c r="Q102" s="11"/>
-      <c r="R102" s="11"/>
-      <c r="S102" s="11"/>
-      <c r="T102" s="11"/>
-      <c r="U102" s="11"/>
-      <c r="V102" s="12"/>
-      <c r="W102" s="12"/>
-    </row>
-    <row r="103" spans="1:23" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="63"/>
-      <c r="B103" s="63"/>
-      <c r="C103" s="63"/>
-      <c r="D103" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E103" s="63"/>
-      <c r="F103" s="63"/>
-      <c r="G103" s="63"/>
-      <c r="H103" s="63"/>
+      <c r="E103" s="50"/>
+      <c r="F103" s="50"/>
+      <c r="G103" s="50"/>
+      <c r="H103" s="50"/>
       <c r="I103" s="11"/>
       <c r="J103" s="11"/>
       <c r="K103" s="11"/>
@@ -4358,7 +4331,7 @@
     </row>
     <row r="104" spans="1:23" ht="53.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="21" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B104" s="22"/>
       <c r="C104" s="22"/>
@@ -4385,15 +4358,15 @@
     </row>
     <row r="105" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="25" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B105" s="22"/>
       <c r="C105" s="22"/>
       <c r="D105" s="6" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="F105" s="28"/>
       <c r="G105" s="28"/>
@@ -4416,7 +4389,7 @@
     </row>
     <row r="106" spans="1:23" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="25" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B106" s="29"/>
       <c r="C106" s="29"/>
@@ -26485,73 +26458,23 @@
       <c r="W1003" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="98">
-    <mergeCell ref="B57:B62"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="A42:A49"/>
-    <mergeCell ref="B42:B49"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="B50:B56"/>
-    <mergeCell ref="B88:B94"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="A88:A94"/>
-    <mergeCell ref="A95:A103"/>
-    <mergeCell ref="B95:B103"/>
-    <mergeCell ref="A73:A79"/>
-    <mergeCell ref="B73:B79"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="A67:A72"/>
-    <mergeCell ref="B67:B72"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="A82:A87"/>
-    <mergeCell ref="B82:B87"/>
-    <mergeCell ref="A57:A62"/>
-    <mergeCell ref="G80:G81"/>
-    <mergeCell ref="H80:H81"/>
-    <mergeCell ref="E67:E72"/>
-    <mergeCell ref="E73:E79"/>
-    <mergeCell ref="F73:F79"/>
-    <mergeCell ref="G73:G79"/>
-    <mergeCell ref="H73:H79"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="F80:F81"/>
-    <mergeCell ref="F67:F72"/>
-    <mergeCell ref="G67:G72"/>
-    <mergeCell ref="H67:H72"/>
-    <mergeCell ref="H88:H94"/>
-    <mergeCell ref="E88:E94"/>
-    <mergeCell ref="E95:E103"/>
-    <mergeCell ref="F95:F103"/>
-    <mergeCell ref="G95:G103"/>
-    <mergeCell ref="H95:H103"/>
-    <mergeCell ref="H42:H49"/>
-    <mergeCell ref="C82:C87"/>
-    <mergeCell ref="C88:C94"/>
-    <mergeCell ref="C95:C103"/>
-    <mergeCell ref="C42:C49"/>
-    <mergeCell ref="C50:C56"/>
-    <mergeCell ref="C57:C62"/>
-    <mergeCell ref="C73:C79"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C67:C72"/>
-    <mergeCell ref="E82:E87"/>
-    <mergeCell ref="F82:F87"/>
-    <mergeCell ref="G82:G87"/>
-    <mergeCell ref="H82:H87"/>
-    <mergeCell ref="F88:F94"/>
-    <mergeCell ref="G88:G94"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="F50:F56"/>
-    <mergeCell ref="F57:F62"/>
-    <mergeCell ref="G57:G62"/>
-    <mergeCell ref="H57:H62"/>
-    <mergeCell ref="E57:E62"/>
-    <mergeCell ref="E63:E66"/>
-    <mergeCell ref="F63:F66"/>
-    <mergeCell ref="G63:G66"/>
-    <mergeCell ref="H63:H66"/>
+  <mergeCells count="91">
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="A9:A41"/>
+    <mergeCell ref="F3:F8"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="B15:B32"/>
+    <mergeCell ref="H15:H32"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="E15:E32"/>
+    <mergeCell ref="F34:F39"/>
+    <mergeCell ref="G34:G39"/>
+    <mergeCell ref="H34:H39"/>
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="A3:A8"/>
     <mergeCell ref="E42:E49"/>
     <mergeCell ref="E50:E56"/>
     <mergeCell ref="G50:G56"/>
@@ -26568,22 +26491,65 @@
     <mergeCell ref="E9:E14"/>
     <mergeCell ref="F42:F49"/>
     <mergeCell ref="G42:G49"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="A9:A41"/>
-    <mergeCell ref="F3:F8"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="B15:B32"/>
-    <mergeCell ref="H15:H32"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="E15:E32"/>
-    <mergeCell ref="F34:F39"/>
-    <mergeCell ref="G34:G39"/>
-    <mergeCell ref="H34:H39"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="F50:F56"/>
+    <mergeCell ref="F57:F62"/>
+    <mergeCell ref="G57:G62"/>
+    <mergeCell ref="H57:H62"/>
+    <mergeCell ref="E57:E62"/>
+    <mergeCell ref="E63:E66"/>
+    <mergeCell ref="F63:F66"/>
+    <mergeCell ref="G63:G66"/>
+    <mergeCell ref="H63:H66"/>
+    <mergeCell ref="H42:H49"/>
+    <mergeCell ref="C82:C87"/>
+    <mergeCell ref="C88:C103"/>
+    <mergeCell ref="C42:C49"/>
+    <mergeCell ref="C50:C56"/>
+    <mergeCell ref="C57:C62"/>
+    <mergeCell ref="C73:C79"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="C67:C72"/>
+    <mergeCell ref="E82:E87"/>
+    <mergeCell ref="F82:F87"/>
+    <mergeCell ref="G82:G87"/>
+    <mergeCell ref="H82:H87"/>
+    <mergeCell ref="F88:F103"/>
+    <mergeCell ref="G88:G103"/>
+    <mergeCell ref="H88:H103"/>
+    <mergeCell ref="E88:E103"/>
+    <mergeCell ref="G80:G81"/>
+    <mergeCell ref="H80:H81"/>
+    <mergeCell ref="E67:E72"/>
+    <mergeCell ref="E73:E79"/>
+    <mergeCell ref="F73:F79"/>
+    <mergeCell ref="G73:G79"/>
+    <mergeCell ref="H73:H79"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="F80:F81"/>
+    <mergeCell ref="F67:F72"/>
+    <mergeCell ref="G67:G72"/>
+    <mergeCell ref="H67:H72"/>
+    <mergeCell ref="B88:B103"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="A88:A103"/>
+    <mergeCell ref="A73:A79"/>
+    <mergeCell ref="B73:B79"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="A67:A72"/>
+    <mergeCell ref="B67:B72"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="A82:A87"/>
+    <mergeCell ref="B82:B87"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="B57:B62"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="A42:A49"/>
+    <mergeCell ref="B42:B49"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="B50:B56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>